<commit_message>
fixed bugs in excel
</commit_message>
<xml_diff>
--- a/UI/bin/Debug/Excel/patternPutOutStorageTicketCover.xlsx
+++ b/UI/bin/Debug/Excel/patternPutOutStorageTicketCover.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17">
   <si>
     <t xml:space="preserve"> @""//套单表，就是打印在已经有表格的纸上的~</t>
   </si>
@@ -33,13 +33,16 @@
     <t>@shipmentTicket.Factory</t>
   </si>
   <si>
-    <t>@putOutStorageTicket.DeliverTime.getFullYear()</t>
-  </si>
-  <si>
-    <t>@putOutStorageTicket.DeliverTime.getMonth()+1</t>
-  </si>
-  <si>
-    <t>@putOutStorageTicket.DeliverTime.getDate()</t>
+    <t>@var time = putOutStorageTicket.DeliverTime;''</t>
+  </si>
+  <si>
+    <t>@time==null?"":time.getFullYear()</t>
+  </si>
+  <si>
+    <t>@time==null?"":time.getMonth()+1</t>
+  </si>
+  <si>
+    <t>@time==null?"":time.getDate()</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -71,11 +74,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -98,6 +101,44 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -105,6 +146,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -120,6 +162,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
@@ -128,7 +178,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -137,36 +187,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -189,6 +209,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -206,37 +240,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -251,187 +254,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,6 +445,50 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -456,6 +503,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -478,67 +540,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -550,10 +553,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -562,133 +565,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1077,7 +1080,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1160,15 +1163,17 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="5"/>
-      <c r="B7" s="8"/>
+      <c r="B7" s="8" t="s">
+        <v>5</v>
+      </c>
       <c r="C7" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="4"/>
@@ -1204,7 +1209,7 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -1223,10 +1228,10 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="4"/>
@@ -1238,19 +1243,19 @@
     </row>
     <row r="13" spans="2:8">
       <c r="B13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>